<commit_message>
pl 2.2, pa2, init pl3
</commit_message>
<xml_diff>
--- a/PL/onedrive/General/ASI-IS2022G41-INFO.xlsx
+++ b/PL/onedrive/General/ASI-IS2022G41-INFO.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo.sharepoint.com/sites/CV22_IngenieradelSoftwareGradoenIngenieraInformticaenTecnolo-IS2022G41/Documentos compartidos/IS2022G41/Archivos Grupo/General/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1100" documentId="8_{0EF9BE6F-0DEF-403D-91E0-274211DB6B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3320D63-6B56-4490-B6C7-5A8D515AB6F5}"/>
+  <xr:revisionPtr revIDLastSave="1129" documentId="8_{0EF9BE6F-0DEF-403D-91E0-274211DB6B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FB7B00F-E0DE-4ED8-9975-570C3926AFA6}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="2190" windowWidth="21600" windowHeight="10020" xr2:uid="{D78DB6CF-6A3C-4D26-819B-E8E504FAD65E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -56,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{9829A219-6AD4-4918-A42B-224F834B8BF1}">
+    <comment ref="F30" authorId="0" shapeId="0" xr:uid="{9829A219-6AD4-4918-A42B-224F834B8BF1}">
       <text>
         <r>
           <rPr>
@@ -71,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F36" authorId="0" shapeId="0" xr:uid="{BB6DAE3D-AB81-4A53-8490-2BFE28F4378A}">
+    <comment ref="F37" authorId="0" shapeId="0" xr:uid="{BB6DAE3D-AB81-4A53-8490-2BFE28F4378A}">
       <text>
         <r>
           <rPr>
@@ -86,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F37" authorId="0" shapeId="0" xr:uid="{DC24F14F-4C1C-4E5B-9021-42B3FBE7608D}">
+    <comment ref="F38" authorId="0" shapeId="0" xr:uid="{DC24F14F-4C1C-4E5B-9021-42B3FBE7608D}">
       <text>
         <r>
           <rPr>
@@ -106,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="85">
   <si>
     <t>Caso de uso</t>
   </si>
@@ -232,6 +233,9 @@
   </si>
   <si>
     <t>Modificar comanda</t>
+  </si>
+  <si>
+    <t>Gestionar comedor</t>
   </si>
   <si>
     <t>Serv. Especiales</t>
@@ -377,12 +381,15 @@
   <si>
     <t>Messi</t>
   </si>
+  <si>
+    <t>freestyle</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,12 +421,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -432,7 +433,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -450,13 +451,8 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -613,13 +609,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -689,17 +706,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
@@ -782,8 +801,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F23105FB-ABFC-465A-85E7-FDEF9E62F42B}" name="Tabla" displayName="Tabla" ref="A2:I69" totalsRowShown="0">
-  <autoFilter ref="A2:I69" xr:uid="{F23105FB-ABFC-465A-85E7-FDEF9E62F42B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F23105FB-ABFC-465A-85E7-FDEF9E62F42B}" name="Tabla" displayName="Tabla" ref="A2:I70" totalsRowShown="0">
+  <autoFilter ref="A2:I70" xr:uid="{F23105FB-ABFC-465A-85E7-FDEF9E62F42B}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{BAF0A4AE-16CF-4E02-8EE4-774DAE06CC9D}" name="Subsistema" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{6811555D-647C-473F-B6EB-CDABC8B863B8}" name="Nombre"/>
@@ -1099,8 +1118,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B43" activeCellId="1" sqref="B42 B43"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1118,13 +1137,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
@@ -1282,7 +1301,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>16</v>
@@ -1309,7 +1328,7 @@
         <v>12</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>16</v>
@@ -1336,7 +1355,7 @@
         <v>12</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>16</v>
@@ -1363,7 +1382,7 @@
         <v>12</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>16</v>
@@ -1763,7 +1782,7 @@
       <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D25" s="10" t="s">
@@ -1786,36 +1805,36 @@
       </c>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="28"/>
+      <c r="B26" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="A27" s="7"/>
       <c r="B27" t="s">
         <v>44</v>
       </c>
@@ -1850,7 +1869,7 @@
         <v>12</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E28" s="10" t="s">
         <v>12</v>
@@ -1878,105 +1897,105 @@
         <v>12</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E29" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F29" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="7"/>
+      <c r="B30" t="s">
         <v>47</v>
       </c>
-      <c r="G29" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="H29" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I29" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="A30" s="1" t="s">
+      <c r="C30" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="G30" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="A31" s="7"/>
-      <c r="B31" t="s">
+      <c r="B31" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F31" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H31" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I31" s="8" t="s">
+      <c r="C31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I31" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="7"/>
       <c r="B32" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>15</v>
-      </c>
       <c r="G32" s="10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1988,7 +2007,7 @@
         <v>12</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E33" s="10" t="s">
         <v>12</v>
@@ -2011,118 +2030,118 @@
       <c r="B34" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F34" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="7"/>
+      <c r="B35" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G34" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I34" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B35" s="2" t="s">
+      <c r="G35" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="7"/>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D36" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F36" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G36" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="H36" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="I36" s="27" t="s">
-        <v>58</v>
+      <c r="D36" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="7"/>
-      <c r="B37" s="28" t="s">
+      <c r="B37" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G37" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="I37" s="12" t="s">
         <v>59</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F37" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="G37" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H37" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I37" s="8" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="7"/>
-      <c r="B38" t="s">
+      <c r="B38" s="27" t="s">
         <v>60</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>15</v>
@@ -2131,16 +2150,14 @@
         <v>12</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>16</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="H38" s="10"/>
       <c r="I38" s="8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -2179,77 +2196,77 @@
         <v>12</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E40" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H40" s="10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I40" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="7"/>
+      <c r="B41" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" s="1" t="s">
+      <c r="C41" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H41" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I41" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B41" s="2" t="s">
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D41" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="7"/>
-      <c r="B42" t="s">
+      <c r="B42" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C42" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F42" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G42" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H42" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I42" s="8" t="s">
+      <c r="C42" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2281,58 +2298,58 @@
       </c>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="13" t="s">
+      <c r="A44" s="7"/>
+      <c r="B44" t="s">
         <v>68</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="C44" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H44" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I44" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C44" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D44" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E44" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F44" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G44" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H44" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I44" s="16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="17"/>
-      <c r="B45" t="s">
+      <c r="B45" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C45" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D45" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F45" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G45" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H45" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I45" s="18" t="s">
+      <c r="C45" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G45" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H45" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I45" s="16" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2431,7 +2448,9 @@
       <c r="E49" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F49" s="10"/>
+      <c r="F49" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="G49" s="10" t="s">
         <v>16</v>
       </c>
@@ -2456,9 +2475,7 @@
       <c r="E50" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F50" s="10" t="s">
-        <v>16</v>
-      </c>
+      <c r="F50" s="10"/>
       <c r="G50" s="10" t="s">
         <v>16</v>
       </c>
@@ -2605,42 +2622,69 @@
       </c>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="19"/>
-      <c r="B56" s="20" t="s">
+      <c r="A56" s="17"/>
+      <c r="B56" t="s">
         <v>81</v>
       </c>
-      <c r="C56" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D56" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E56" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="F56" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G56" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H56" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I56" s="22" t="s">
+      <c r="C56" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G56" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H56" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I56" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="19"/>
+      <c r="B57" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C57" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E57" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G57" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="H57" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="I57" s="22" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="136" spans="10:10">
       <c r="J136" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:F1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A3:I56">
+  <conditionalFormatting sqref="A3:I57">
     <cfRule type="beginsWith" dxfId="10" priority="3" operator="beginsWith" text="-">
       <formula>LEFT(A3,LEN("-"))="-"</formula>
     </cfRule>
@@ -2651,7 +2695,7 @@
       <formula>NOT(ISERROR(SEARCH("NO",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F56">
+  <conditionalFormatting sqref="F3:F57">
     <cfRule type="containsText" priority="1" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",F3)))</formula>
     </cfRule>
@@ -2665,13 +2709,40 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B85370B-0A58-4996-9305-45FA9A979E6C}">
+  <dimension ref="Y54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="54" spans="25:25">
+      <c r="Y54" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001DAE15A8A044AF4C90B2C91A396E124F" ma:contentTypeVersion="8" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="c841cb3c5775b460c8cdab70c33efac6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fecce1b3-694a-4a80-9daa-87b4ccfff5b9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="832f6480a4c6f8aaecbe7cd77ea70b4a" ns2:_="">
     <xsd:import namespace="fecce1b3-694a-4a80-9daa-87b4ccfff5b9"/>
@@ -2823,23 +2894,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9752B53C-4B29-413B-AD73-896FBC4E8238}"/>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4680E689-075A-46C0-AD8A-E3C26FB1AC4A}"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F8FE195-4027-40B7-B73D-73D9308669A5}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9752B53C-4B29-413B-AD73-896FBC4E8238}"/>
 </file>
</xml_diff>